<commit_message>
add new meta data files
</commit_message>
<xml_diff>
--- a/data/raw/public/f_chicagoGreenSpace_1/DEC_10_PL_P2_metadata.xlsx
+++ b/data/raw/public/f_chicagoGreenSpace_1/DEC_10_PL_P2_metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QGISProjects\f_chicagoNature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaiahbennett/Documents/Chicago-green-space-final/data/raw/public/f_chicagoGreenSpace_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07E499A-E41F-1646-A169-C7C700DF0D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33570" windowHeight="15500"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEC_10_PL_P2_metadata" sheetId="1" r:id="rId1"/>
@@ -480,8 +481,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +619,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -968,7 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1289,16 +1296,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="73.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1322,7 +1332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1340,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1338,7 +1348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1346,7 +1356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1362,7 +1372,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1370,7 +1380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1386,7 +1396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1394,7 +1404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1402,7 +1412,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1410,7 +1420,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1418,7 +1428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1426,7 +1436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1434,7 +1444,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1442,7 +1452,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1466,7 +1476,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1474,7 +1484,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1482,7 +1492,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1490,7 +1500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1498,7 +1508,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1514,7 +1524,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1522,7 +1532,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1530,7 +1540,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1538,7 +1548,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -1546,7 +1556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1554,7 +1564,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -1562,7 +1572,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1570,7 +1580,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -1578,7 +1588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -1586,7 +1596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -1594,7 +1604,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -1602,7 +1612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -1610,7 +1620,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1618,7 +1628,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -1626,7 +1636,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -1634,7 +1644,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -1642,7 +1652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -1650,7 +1660,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -1658,7 +1668,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -1666,7 +1676,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1674,7 +1684,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -1682,7 +1692,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -1690,7 +1700,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -1698,7 +1708,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1706,7 +1716,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -1714,7 +1724,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -1722,7 +1732,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -1738,7 +1748,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -1746,7 +1756,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>111</v>
       </c>
@@ -1754,7 +1764,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>113</v>
       </c>
@@ -1762,7 +1772,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>115</v>
       </c>
@@ -1770,7 +1780,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -1778,7 +1788,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -1786,7 +1796,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>121</v>
       </c>
@@ -1794,7 +1804,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -1802,7 +1812,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>125</v>
       </c>
@@ -1810,7 +1820,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>127</v>
       </c>
@@ -1818,7 +1828,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>129</v>
       </c>
@@ -1826,7 +1836,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -1834,7 +1844,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -1842,7 +1852,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>135</v>
       </c>
@@ -1850,7 +1860,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>137</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>139</v>
       </c>
@@ -1866,7 +1876,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>141</v>
       </c>
@@ -1874,7 +1884,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>143</v>
       </c>
@@ -1882,7 +1892,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -1890,7 +1900,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>147</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>149</v>
       </c>
@@ -1907,6 +1917,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>